<commit_message>
- Remove temp record folder - Folder tidy
</commit_message>
<xml_diff>
--- a/bin/configuration.xlsx
+++ b/bin/configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimke\OneDrive\Documents\investment and trading\stocks and equity\sandbox\WealthAndFreedom\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae26920bfc737752/Documents/investment and trading/stocks and equity/sandbox/WealthAndFreedom/bin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{AE6025BF-8A51-4B7E-BC9A-073966384CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAA0A2F7-3841-40DC-BFBD-5740012DC5EF}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AE6025BF-8A51-4B7E-BC9A-073966384CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EA1427B-9CEF-4445-A935-52DAF131B5E0}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="3900" windowWidth="27870" windowHeight="5820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6375" yWindow="15615" windowWidth="27870" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="moving_price" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>Events</t>
   </si>
   <si>
-    <t>Public Holiday</t>
+    <t>public holiday</t>
   </si>
 </sst>
 </file>
@@ -33422,8 +33422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9779B97-5761-460A-9B2C-248D248ED206}">
   <dimension ref="A1:D2199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1821" workbookViewId="0">
-      <selection activeCell="D1850" sqref="D1850"/>
+    <sheetView tabSelected="1" topLeftCell="A964" workbookViewId="0">
+      <selection activeCell="G967" sqref="G967"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -62002,7 +62002,7 @@
         <v>44185</v>
       </c>
       <c r="C2178" s="3" t="str">
-        <f t="shared" ref="C2178:C2241" si="68">IF(OR(WEEKDAY(A2178,2)&gt;=6, NOT(ISBLANK(D2178))), "Close", "Open")</f>
+        <f t="shared" ref="C2178:C2199" si="68">IF(OR(WEEKDAY(A2178,2)&gt;=6, NOT(ISBLANK(D2178))), "Close", "Open")</f>
         <v>Close</v>
       </c>
     </row>

</xml_diff>